<commit_message>
added normalisation + erd to application fact sheet + making data dictionary
</commit_message>
<xml_diff>
--- a/Coursework/Database Analysis and Design/Normalisation.xlsx
+++ b/Coursework/Database Analysis and Design/Normalisation.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20348"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jharrison12\ISAD251\Coursework\Database Analysis and Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC269C4C-6D67-4041-9027-087E9D1EC634}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="110">
   <si>
     <t>UNF</t>
   </si>
@@ -253,37 +257,107 @@
   </si>
   <si>
     <t>DATETIME</t>
+  </si>
+  <si>
+    <t>CustomerFirstName</t>
+  </si>
+  <si>
+    <t>ProductOrderPrice</t>
+  </si>
+  <si>
+    <t>OrderTotalPrice</t>
+  </si>
+  <si>
+    <t>ProductOrderQuantity</t>
+  </si>
+  <si>
+    <t>OrderTotalPrice)</t>
+  </si>
+  <si>
+    <t>ProductID*</t>
+  </si>
+  <si>
+    <t>OrderID*</t>
+  </si>
+  <si>
+    <t>CustomerID*</t>
+  </si>
+  <si>
+    <t>DATA DICTIONARY</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>Field Size</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>First name for customer</t>
+  </si>
+  <si>
+    <t>Unique ID for customer</t>
+  </si>
+  <si>
+    <t>Surname for customer</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>CustomerSurname</t>
+  </si>
+  <si>
+    <t>Customersurname</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Unique ID for order</t>
+  </si>
+  <si>
+    <t>Date of order</t>
+  </si>
+  <si>
+    <t>Total price of order</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>NNNNN</t>
+  </si>
+  <si>
+    <t>xxx.xx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -305,6 +379,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -346,17 +428,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,6 +455,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -414,7 +506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,9 +539,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,6 +591,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -657,1994 +783,2389 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J161"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L147" sqref="L147"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E208" sqref="E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="7" width="27.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="6"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F60" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F63" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="F67" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F68" s="6"/>
+      <c r="F68" s="3"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F72" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="F78" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E79" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F81" s="8" t="s">
+      <c r="F81" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E82" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E83" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E84" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E87" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F89" s="6" t="s">
+      <c r="F89" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F92" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E94" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E95" s="3"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F96" s="6" t="s">
+      <c r="F96" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E97" s="4" t="s">
+      <c r="E97" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F97" s="6"/>
+      <c r="F97" s="3"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E100" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F100" s="6" t="s">
+      <c r="F100" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E101" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E102" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E103" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C104" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D104" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E104" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D105" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E105" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E108" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E109" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E111" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E112" s="3" t="s">
+      <c r="E112" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E115" s="3" t="s">
+      <c r="E115" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B118" s="7" t="s">
+      <c r="B118" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D118" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E118" s="7" t="s">
+      <c r="E118" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F118" s="7" t="s">
+      <c r="F118" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I118" s="9" t="s">
+      <c r="I118" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="J118" s="9" t="s">
+      <c r="J118" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E120" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F120" s="6" t="s">
+      <c r="F120" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I120" s="5" t="s">
+      <c r="I120" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J120" s="5" t="s">
+      <c r="J120" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I121" s="5" t="s">
+      <c r="I121" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J121" t="s">
+      <c r="J121" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I122" s="5" t="s">
+      <c r="I122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J122" t="s">
+      <c r="J122" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I123" s="5" t="s">
+      <c r="I123" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J123" t="s">
+      <c r="J123" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I124" s="5" t="s">
+      <c r="I124" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J124" t="s">
+      <c r="J124" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I125" s="3" t="s">
+      <c r="I125" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J125" t="s">
+      <c r="J125" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E126" s="4" t="s">
+      <c r="E126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F126" s="6" t="s">
+      <c r="F126" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I126" s="3" t="s">
+      <c r="I126" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J126" t="s">
+      <c r="J126" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D127" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E127" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I127" s="3" t="s">
+      <c r="I127" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J127" t="s">
+      <c r="J127" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I128" s="3" t="s">
+      <c r="I128" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J128" t="s">
+      <c r="J128" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I129" s="3" t="s">
+      <c r="I129" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J129" t="s">
+      <c r="J129" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="E130" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I130" s="3" t="s">
+      <c r="I130" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J130" t="s">
+      <c r="J130" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D131" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E131" s="3" t="s">
+      <c r="E131" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I131" s="3" t="s">
+      <c r="I131" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J131" t="s">
+      <c r="J131" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C132" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E132" s="3" t="s">
+      <c r="E132" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I132" s="3" t="s">
+      <c r="I132" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J132" t="s">
+      <c r="J132" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="C133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E133" s="3" t="s">
+      <c r="E133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I133" s="3" t="s">
+      <c r="I133" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J133" t="s">
+      <c r="J133" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="C134" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E134" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I134" s="3" t="s">
+      <c r="I134" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J134" t="s">
+      <c r="J134" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="C135" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D135" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E135" s="3" t="s">
+      <c r="E135" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I135" s="3" t="s">
+      <c r="I135" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J135" t="s">
+      <c r="J135" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I136" s="3" t="s">
+      <c r="I136" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J136" t="s">
+      <c r="J136" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="E137" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F137" s="6" t="s">
+      <c r="F137" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I137" s="3" t="s">
+      <c r="I137" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J137" t="s">
+      <c r="J137" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I138" s="3" t="s">
+      <c r="I138" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J138" t="s">
+      <c r="J138" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="139" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="C139" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E139" s="3" t="s">
+      <c r="E139" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I139" s="3" t="s">
+      <c r="I139" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J139" t="s">
+      <c r="J139" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="140" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C140" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D140" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E140" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F140" s="6"/>
-      <c r="I140" s="3" t="s">
+      <c r="F140" s="3"/>
+      <c r="I140" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J140" t="s">
+      <c r="J140" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="141" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C141" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I141" s="3" t="s">
+      <c r="I141" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J141" t="s">
+      <c r="J141" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="142" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C142" s="3" t="s">
+      <c r="C142" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E142" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F142" s="6" t="s">
+      <c r="F142" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I142" s="3" t="s">
+      <c r="I142" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J142" t="s">
+      <c r="J142" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="143" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D143" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E143" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F143" s="6"/>
-      <c r="I143" s="3" t="s">
+      <c r="F143" s="3"/>
+      <c r="I143" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J143" t="s">
+      <c r="J143" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="144" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E144" s="3" t="s">
+      <c r="E144" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I144" s="3" t="s">
+      <c r="I144" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J144" t="s">
+      <c r="J144" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="145" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C145" s="3" t="s">
+      <c r="C145" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I145" s="3" t="s">
+      <c r="I145" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J145" t="s">
+      <c r="J145" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="146" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C146" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D146" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E146" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F146" s="6" t="s">
+      <c r="F146" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I146" s="3" t="s">
+      <c r="I146" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J146" t="s">
+      <c r="J146" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="147" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B147" s="2" t="s">
+      <c r="B147" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C147" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E147" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I147" s="3" t="s">
+      <c r="I147" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J147" t="s">
+      <c r="J147" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="148" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B148" s="2" t="s">
+      <c r="B148" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C148" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E148" s="3" t="s">
+      <c r="E148" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I148" s="3" t="s">
+      <c r="I148" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J148" t="s">
+      <c r="J148" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="149" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C149" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E149" s="3" t="s">
+      <c r="E149" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I149" s="3" t="s">
+      <c r="I149" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J149" t="s">
+      <c r="J149" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="150" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C150" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D150" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E150" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I150" s="3" t="s">
+      <c r="I150" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J150" t="s">
+      <c r="J150" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="151" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C151" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E151" s="3" t="s">
+      <c r="E151" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I151" s="3" t="s">
+      <c r="I151" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J151" t="s">
+      <c r="J151" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="152" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C152" s="3" t="s">
+      <c r="C152" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D152" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E152" s="3" t="s">
+      <c r="E152" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="153" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="3" t="s">
+      <c r="C153" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D153" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E153" s="3" t="s">
+      <c r="E153" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="154" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C154" s="3" t="s">
+      <c r="C154" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E154" s="3" t="s">
+      <c r="E154" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="155" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C155" s="3" t="s">
+      <c r="C155" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D155" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E155" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="156" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C156" s="3" t="s">
+      <c r="C156" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D156" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E156" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="157" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C157" s="3" t="s">
+      <c r="C157" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E157" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="158" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D158" s="3" t="s">
+      <c r="D158" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E158" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="159" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D159" s="3" t="s">
+      <c r="D159" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E159" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="160" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E160" s="3" t="s">
+      <c r="E160" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E161" s="3" t="s">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E161" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B165" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B167" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B171" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B172" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B173" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B174" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B175" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B176" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F176" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B177" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B178" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B179" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B180" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C181" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F181" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C182" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C183" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D184" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D185" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F185" s="3"/>
+    </row>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E186" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F187" s="3"/>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B189" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D189" s="2"/>
+      <c r="E189" s="2"/>
+      <c r="F189" s="3"/>
+    </row>
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E190" s="2"/>
+      <c r="F190" s="3"/>
+    </row>
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C191" s="2"/>
+    </row>
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B192" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F192" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G192" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B193" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E193" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F193" s="8">
+        <v>5</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H193" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C194" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E194" s="8"/>
+      <c r="F194" s="8">
+        <v>20</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H194" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C195" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E195" s="8"/>
+      <c r="F195" s="8">
+        <v>20</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B196" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E196" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F196" s="8">
+        <v>5</v>
+      </c>
+      <c r="G196" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H196" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C197" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F197" s="8">
+        <v>10</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H197" s="10">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C198" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E198" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F198" s="8">
+        <v>5</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H198" s="8">
+        <v>13.99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>